<commit_message>
temp reader - first commit
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas Pozzi\Documents\Dev\manual-compiler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lferreira25\Documents\manual-compiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A572D548-31B0-4545-9D36-F9B56B1152AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BC1686-3804-4F86-AC4E-3A23CB7242D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28035" yWindow="5850" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,24 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>type</t>
   </si>
   <si>
-    <t>DIR</t>
-  </si>
-  <si>
-    <t>CAD</t>
-  </si>
-  <si>
-    <t>PDC</t>
-  </si>
-  <si>
     <t>file</t>
-  </si>
-  <si>
-    <t>converted document</t>
   </si>
   <si>
     <t>version</t>
@@ -84,8 +72,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,34 +355,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
+      <c r="B2" s="1">
+        <v>100014616490</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -403,31 +392,26 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="B3" s="1">
+        <v>100033325020</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 SLB-Private</oddFooter>
+  </headerFooter>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{8bb759f6-5337-4dc5-b19b-e74b6da11f8f}" enabled="1" method="Standard" siteId="{41ff26dc-250f-4b13-8981-739be8610c21}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Back opps - organization
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lferreira25\Documents\manual-compiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BC1686-3804-4F86-AC4E-3A23CB7242D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD149A57-DA0E-4D07-A253-BCAAAEB629F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28035" yWindow="5850" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="4560" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,282 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>file</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="92">
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>new version</t>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>Sensores</t>
+  </si>
+  <si>
+    <t>Sensor de pressão de formação</t>
+  </si>
+  <si>
+    <t>SLB_sensor_001</t>
+  </si>
+  <si>
+    <t>v1.0</t>
+  </si>
+  <si>
+    <t>Sensor de densidade de fluido</t>
+  </si>
+  <si>
+    <t>SLB_sensor_002</t>
+  </si>
+  <si>
+    <t>Sensor de salinidade de água</t>
+  </si>
+  <si>
+    <t>SLB_sensor_003</t>
+  </si>
+  <si>
+    <t>Sensor de concentração de gás</t>
+  </si>
+  <si>
+    <t>SLB_sensor_004</t>
+  </si>
+  <si>
+    <t>Sensor de viscosidade de fluido</t>
+  </si>
+  <si>
+    <t>SLB_sensor_005</t>
+  </si>
+  <si>
+    <t>Sensor de temperatura de formação</t>
+  </si>
+  <si>
+    <t>SLB_sensor_006</t>
+  </si>
+  <si>
+    <t>Sensor de nível de líquido</t>
+  </si>
+  <si>
+    <t>SLB_sensor_007</t>
+  </si>
+  <si>
+    <t>Sensor de concentração de água</t>
+  </si>
+  <si>
+    <t>SLB_sensor_008</t>
+  </si>
+  <si>
+    <t>Sensor de pressão de superfície</t>
+  </si>
+  <si>
+    <t>SLB_sensor_009</t>
+  </si>
+  <si>
+    <t>Sensor de temperatura de poço</t>
+  </si>
+  <si>
+    <t>SLB_sensor_010</t>
+  </si>
+  <si>
+    <t>Ferramentas</t>
+  </si>
+  <si>
+    <t>Ferramenta de perfilagem de poço</t>
+  </si>
+  <si>
+    <t>SLB_tool_011</t>
+  </si>
+  <si>
+    <t>Ferramenta de medição de temperatura</t>
+  </si>
+  <si>
+    <t>SLB_tool_012</t>
+  </si>
+  <si>
+    <t>Ferramenta de medição de vazão</t>
+  </si>
+  <si>
+    <t>SLB_tool_013</t>
+  </si>
+  <si>
+    <t>Ferramenta de perfuração direcional</t>
+  </si>
+  <si>
+    <t>SLB_tool_014</t>
+  </si>
+  <si>
+    <t>Ferramenta de amostragem de fluido</t>
+  </si>
+  <si>
+    <t>SLB_tool_015</t>
+  </si>
+  <si>
+    <t>Ferramenta de teste de formação</t>
+  </si>
+  <si>
+    <t>SLB_tool_016</t>
+  </si>
+  <si>
+    <t>Ferramenta de recuperação secundária</t>
+  </si>
+  <si>
+    <t>SLB_tool_017</t>
+  </si>
+  <si>
+    <t>Ferramenta de estimulação de poço</t>
+  </si>
+  <si>
+    <t>SLB_tool_018</t>
+  </si>
+  <si>
+    <t>Ferramenta de perfuração rotativa</t>
+  </si>
+  <si>
+    <t>SLB_tool_019</t>
+  </si>
+  <si>
+    <t>Ferramenta de perfilagem elétrica</t>
+  </si>
+  <si>
+    <t>SLB_tool_020</t>
+  </si>
+  <si>
+    <t>Sistemas</t>
+  </si>
+  <si>
+    <t>Sistema de controle de cabeçote de poço</t>
+  </si>
+  <si>
+    <t>SLB_system_021</t>
+  </si>
+  <si>
+    <t>Sistema de completação inteligente</t>
+  </si>
+  <si>
+    <t>SLB_system_022</t>
+  </si>
+  <si>
+    <t>Sistema de monitoramento de poço</t>
+  </si>
+  <si>
+    <t>SLB_system_023</t>
+  </si>
+  <si>
+    <t>Sistema de injeção de água</t>
+  </si>
+  <si>
+    <t>SLB_system_024</t>
+  </si>
+  <si>
+    <t>Sistema de controle de produção</t>
+  </si>
+  <si>
+    <t>SLB_system_025</t>
+  </si>
+  <si>
+    <t>Sistema de medição de vazão multifásica</t>
+  </si>
+  <si>
+    <t>SLB_system_026</t>
+  </si>
+  <si>
+    <t>Sistema de controle de completação</t>
+  </si>
+  <si>
+    <t>SLB_system_027</t>
+  </si>
+  <si>
+    <t>Sistema de controle de produção submarina</t>
+  </si>
+  <si>
+    <t>SLB_system_028</t>
+  </si>
+  <si>
+    <t>Sistema de controle de formação</t>
+  </si>
+  <si>
+    <t>SLB_system_029</t>
+  </si>
+  <si>
+    <t>Sistema de injeção química</t>
+  </si>
+  <si>
+    <t>SLB_system_030</t>
+  </si>
+  <si>
+    <t>Válvulas</t>
+  </si>
+  <si>
+    <t>Válvula de segurança de superfície</t>
+  </si>
+  <si>
+    <t>SLB_valve_031</t>
+  </si>
+  <si>
+    <t>Válvula de controle de fluxo</t>
+  </si>
+  <si>
+    <t>SLB_valve_032</t>
+  </si>
+  <si>
+    <t>Válvula de retenção de pressão</t>
+  </si>
+  <si>
+    <t>SLB_valve_033</t>
+  </si>
+  <si>
+    <t>Válvula de controle de pressão</t>
+  </si>
+  <si>
+    <t>SLB_valve_034</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Capa</t>
+  </si>
+  <si>
+    <t>Apresentação</t>
+  </si>
+  <si>
+    <t>$Bookmark_general</t>
+  </si>
+  <si>
+    <t>$Bookmark_description</t>
+  </si>
+  <si>
+    <t>DIR/PN</t>
+  </si>
+  <si>
+    <t>$Bookmark_dirpn</t>
+  </si>
+  <si>
+    <t>$Bookmark_sensores</t>
+  </si>
+  <si>
+    <t>$Bookmark_Ferramentas</t>
+  </si>
+  <si>
+    <t>$Bookmark_Sistemas</t>
+  </si>
+  <si>
+    <t>$Bookmark_Válvulas</t>
+  </si>
+  <si>
+    <t>subsection</t>
+  </si>
+  <si>
+    <t>Pressão e densidade</t>
+  </si>
+  <si>
+    <t>Nível</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -355,51 +619,597 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="4" width="30.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1">
-        <v>100014616490</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
-        <v>100033325020</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" t="s">
+        <v>63</v>
+      </c>
+      <c r="F37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E43" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E44" t="s">
+        <v>76</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Back opps - version test
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lferreira25\Documents\manual-compiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD149A57-DA0E-4D07-A253-BCAAAEB629F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFA57A7-BCB9-4E02-8BC1-1FC055516EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4560" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="100">
   <si>
     <t>version</t>
   </si>
@@ -301,6 +312,30 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>Cover</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>$summary</t>
+  </si>
+  <si>
+    <t>$index_section</t>
+  </si>
+  <si>
+    <t>$index_description</t>
+  </si>
+  <si>
+    <t>$index_dirpn</t>
+  </si>
+  <si>
+    <t>Fluxograma Geral _ Lista de Pesos e Dimensões _ Controle de Revisões</t>
+  </si>
+  <si>
+    <t>$index_section_local</t>
   </si>
 </sst>
 </file>
@@ -619,596 +654,685 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="B1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A9" sqref="A9:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="4" width="30.7109375" style="1" customWidth="1"/>
-    <col min="5" max="6" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="5" width="30.7109375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G71" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="I71" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G72" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="I72" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G73" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+    </row>
+    <row r="75" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+    </row>
+    <row r="76" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+    </row>
+    <row r="77" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G77" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
+      <c r="H77" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="I77" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E8" t="s">
+      <c r="J77" s="1"/>
+      <c r="K77" t="s">
         <v>6</v>
       </c>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="L77" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G78" t="s">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
+      <c r="H78" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="I78" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+      <c r="J78" s="1"/>
+      <c r="K78" t="s">
         <v>9</v>
       </c>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="L78" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G79" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
+      <c r="H79" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="I79" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E10" t="s">
+      <c r="J79" s="1"/>
+      <c r="K79" t="s">
         <v>11</v>
       </c>
-      <c r="F10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="L79" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G80" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
+      <c r="H80" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="I80" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E11" t="s">
+      <c r="J80" s="1"/>
+      <c r="K80" t="s">
         <v>13</v>
       </c>
-      <c r="F11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="L80" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G81" t="s">
         <v>4</v>
       </c>
-      <c r="B12" t="s">
+      <c r="H81" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="I81" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E12" t="s">
+      <c r="J81" s="1"/>
+      <c r="K81" t="s">
         <v>15</v>
       </c>
-      <c r="F12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="L81" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G82" t="s">
         <v>4</v>
       </c>
-      <c r="B13" t="s">
+      <c r="H82" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="I82" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
+      <c r="J82" s="1"/>
+      <c r="K82" t="s">
         <v>17</v>
       </c>
-      <c r="F13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="L82" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G83" t="s">
         <v>4</v>
       </c>
-      <c r="B14" t="s">
+      <c r="H83" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="I83" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E14" t="s">
+      <c r="J83" s="1"/>
+      <c r="K83" t="s">
         <v>19</v>
       </c>
-      <c r="F14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="L83" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G84" t="s">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
+      <c r="H84" t="s">
         <v>90</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="I84" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E15" t="s">
+      <c r="J84" s="1"/>
+      <c r="K84" t="s">
         <v>21</v>
       </c>
-      <c r="F15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="L84" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G85" t="s">
         <v>4</v>
       </c>
-      <c r="B16" t="s">
+      <c r="H85" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="I85" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E16" t="s">
+      <c r="J85" s="1"/>
+      <c r="K85" t="s">
         <v>23</v>
       </c>
-      <c r="F16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="L85" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G86" t="s">
         <v>4</v>
       </c>
-      <c r="B17" t="s">
+      <c r="H86" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="I86" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E17" t="s">
+      <c r="J86" s="1"/>
+      <c r="K86" t="s">
         <v>25</v>
       </c>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="L86" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G87" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+    </row>
+    <row r="88" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G88" t="s">
         <v>26</v>
       </c>
-      <c r="B19" t="s">
+      <c r="H88" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="I88" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E19" t="s">
+      <c r="J88" s="1"/>
+      <c r="K88" t="s">
         <v>28</v>
       </c>
-      <c r="F19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="L88" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G89" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="I89" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E20" t="s">
+      <c r="J89" s="1"/>
+      <c r="K89" t="s">
         <v>30</v>
       </c>
-      <c r="F20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="L89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G90" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="I90" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E21" t="s">
+      <c r="J90" s="1"/>
+      <c r="K90" t="s">
         <v>32</v>
       </c>
-      <c r="F21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="L90" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G91" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="I91" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E22" t="s">
+      <c r="J91" s="1"/>
+      <c r="K91" t="s">
         <v>34</v>
       </c>
-      <c r="F22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="L91" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G92" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="I92" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E23" t="s">
+      <c r="J92" s="1"/>
+      <c r="K92" t="s">
         <v>36</v>
       </c>
-      <c r="F23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="L92" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G93" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="I93" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E24" t="s">
+      <c r="J93" s="1"/>
+      <c r="K93" t="s">
         <v>38</v>
       </c>
-      <c r="F24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="L93" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G94" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="I94" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E25" t="s">
+      <c r="J94" s="1"/>
+      <c r="K94" t="s">
         <v>40</v>
       </c>
-      <c r="F25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="L94" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G95" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="I95" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E26" t="s">
+      <c r="J95" s="1"/>
+      <c r="K95" t="s">
         <v>42</v>
       </c>
-      <c r="F26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="L95" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G96" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="I96" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E27" t="s">
+      <c r="J96" s="1"/>
+      <c r="K96" t="s">
         <v>44</v>
       </c>
-      <c r="F27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="L96" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G97" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="I97" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E28" t="s">
+      <c r="J97" s="1"/>
+      <c r="K97" t="s">
         <v>46</v>
       </c>
-      <c r="F28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="L97" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G98" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+    </row>
+    <row r="99" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G99" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="I99" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E30" t="s">
+      <c r="J99" s="1"/>
+      <c r="K99" t="s">
         <v>49</v>
       </c>
-      <c r="F30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="L99" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G100" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="I100" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E31" t="s">
+      <c r="J100" s="1"/>
+      <c r="K100" t="s">
         <v>51</v>
       </c>
-      <c r="F31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="L100" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G101" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="I101" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E32" t="s">
+      <c r="J101" s="1"/>
+      <c r="K101" t="s">
         <v>53</v>
       </c>
-      <c r="F32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="L101" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G102" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="I102" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E33" t="s">
+      <c r="J102" s="1"/>
+      <c r="K102" t="s">
         <v>55</v>
       </c>
-      <c r="F33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="L102" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G103" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="I103" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E34" t="s">
+      <c r="J103" s="1"/>
+      <c r="K103" t="s">
         <v>57</v>
       </c>
-      <c r="F34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="L103" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="I104" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E35" t="s">
+      <c r="J104" s="1"/>
+      <c r="K104" t="s">
         <v>59</v>
       </c>
-      <c r="F35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="L104" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G105" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="I105" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E36" t="s">
+      <c r="J105" s="1"/>
+      <c r="K105" t="s">
         <v>61</v>
       </c>
-      <c r="F36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="L105" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G106" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="I106" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E37" t="s">
+      <c r="J106" s="1"/>
+      <c r="K106" t="s">
         <v>63</v>
       </c>
-      <c r="F37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="L106" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G107" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="I107" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E38" t="s">
+      <c r="J107" s="1"/>
+      <c r="K107" t="s">
         <v>65</v>
       </c>
-      <c r="F38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="L107" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G108" t="s">
         <v>47</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="I108" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E39" t="s">
+      <c r="J108" s="1"/>
+      <c r="K108" t="s">
         <v>67</v>
       </c>
-      <c r="F39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="L108" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G109" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="I109" s="1"/>
+      <c r="J109" s="1"/>
+    </row>
+    <row r="110" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G110" t="s">
         <v>68</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="I110" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E41" t="s">
+      <c r="J110" s="1"/>
+      <c r="K110" t="s">
         <v>70</v>
       </c>
-      <c r="F41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="L110" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G111" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="I111" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E42" t="s">
+      <c r="J111" s="1"/>
+      <c r="K111" t="s">
         <v>72</v>
       </c>
-      <c r="F42" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="L111" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G112" t="s">
         <v>68</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="I112" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E43" t="s">
+      <c r="J112" s="1"/>
+      <c r="K112" t="s">
         <v>74</v>
       </c>
-      <c r="F43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="L112" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G113" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="I113" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E44" t="s">
+      <c r="J113" s="1"/>
+      <c r="K113" t="s">
         <v>76</v>
       </c>
-      <c r="F44" t="s">
+      <c r="L113" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>